<commit_message>
A few corrections on instances
</commit_message>
<xml_diff>
--- a/Dataset/GECCO19.xlsx
+++ b/Dataset/GECCO19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\PhD\PhD\github\CSPLib\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C8361-730B-41FC-8F51-2917F60FC837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B233FB36-F5C7-496B-9171-5DE2E99797E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1238,9 +1238,6 @@
     <t>person128</t>
   </si>
   <si>
-    <t>person30, person34, person62, person79, person148, person129</t>
-  </si>
-  <si>
     <t>person180, person130</t>
   </si>
   <si>
@@ -1521,6 +1518,9 @@
   </si>
   <si>
     <t>Forum Hall</t>
+  </si>
+  <si>
+    <t>person30, person34, person62. person79, person148, person129</t>
   </si>
 </sst>
 </file>
@@ -1987,7 +1987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -2199,9 +2199,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C69255-5912-4D6E-83E6-D37C87DA9D15}">
   <dimension ref="A1:AD203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2240,37 +2240,37 @@
         <v>29</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>475</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>478</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>479</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>481</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>482</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>483</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>484</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>485</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>30</v>
@@ -2279,34 +2279,34 @@
         <v>31</v>
       </c>
       <c r="U1" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="V1" s="26" t="s">
         <v>486</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>487</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="X1" s="26" t="s">
         <v>488</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="Y1" s="26" t="s">
         <v>489</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>490</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>491</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>492</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AC1" s="26" t="s">
         <v>493</v>
       </c>
-      <c r="AC1" s="26" t="s">
+      <c r="AD1" s="26" t="s">
         <v>494</v>
-      </c>
-      <c r="AD1" s="26" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2923,6 +2923,7 @@
       <c r="F19" s="16" t="s">
         <v>290</v>
       </c>
+      <c r="G19" s="16"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
@@ -2956,6 +2957,7 @@
       <c r="F20" s="16" t="s">
         <v>291</v>
       </c>
+      <c r="G20" s="16"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
@@ -2989,6 +2991,7 @@
       <c r="F21" s="16" t="s">
         <v>292</v>
       </c>
+      <c r="G21" s="16"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
@@ -3022,6 +3025,7 @@
       <c r="F22" s="16" t="s">
         <v>293</v>
       </c>
+      <c r="G22" s="16"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
@@ -3055,6 +3059,7 @@
       <c r="F23" s="16" t="s">
         <v>294</v>
       </c>
+      <c r="G23" s="16"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
@@ -3224,6 +3229,7 @@
       <c r="F28" s="16" t="s">
         <v>299</v>
       </c>
+      <c r="G28" s="16"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
@@ -3257,6 +3263,7 @@
       <c r="F29" s="16" t="s">
         <v>300</v>
       </c>
+      <c r="G29" s="16"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
@@ -3290,6 +3297,7 @@
       <c r="F30" s="16" t="s">
         <v>301</v>
       </c>
+      <c r="G30" s="16"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
@@ -3323,6 +3331,7 @@
       <c r="F31" s="16" t="s">
         <v>302</v>
       </c>
+      <c r="G31" s="16"/>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
@@ -3356,6 +3365,7 @@
       <c r="F32" s="16" t="s">
         <v>303</v>
       </c>
+      <c r="G32" s="16"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
       <c r="N32" s="15"/>
@@ -3491,6 +3501,7 @@
       <c r="F36" s="16" t="s">
         <v>307</v>
       </c>
+      <c r="G36" s="16"/>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
@@ -3592,6 +3603,7 @@
       <c r="F39" s="16" t="s">
         <v>310</v>
       </c>
+      <c r="G39" s="16"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
@@ -3623,6 +3635,7 @@
       <c r="F40" s="16" t="s">
         <v>311</v>
       </c>
+      <c r="G40" s="16"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
@@ -3654,6 +3667,7 @@
       <c r="F41" s="16" t="s">
         <v>312</v>
       </c>
+      <c r="G41" s="16"/>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
@@ -3685,6 +3699,7 @@
       <c r="F42" s="16" t="s">
         <v>313</v>
       </c>
+      <c r="G42" s="16"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
@@ -3716,6 +3731,7 @@
       <c r="F43" s="16" t="s">
         <v>314</v>
       </c>
+      <c r="G43" s="16"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
@@ -3747,6 +3763,7 @@
       <c r="F44" s="16" t="s">
         <v>315</v>
       </c>
+      <c r="G44" s="16"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
@@ -3778,6 +3795,7 @@
       <c r="F45" s="16" t="s">
         <v>316</v>
       </c>
+      <c r="G45" s="16"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
@@ -3809,6 +3827,7 @@
       <c r="F46" s="16" t="s">
         <v>317</v>
       </c>
+      <c r="G46" s="16"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
@@ -3840,6 +3859,7 @@
       <c r="F47" s="16" t="s">
         <v>318</v>
       </c>
+      <c r="G47" s="16"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
@@ -3871,6 +3891,7 @@
       <c r="F48" s="16" t="s">
         <v>319</v>
       </c>
+      <c r="G48" s="16"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
@@ -3902,6 +3923,7 @@
       <c r="F49" s="16" t="s">
         <v>320</v>
       </c>
+      <c r="G49" s="16"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
@@ -3933,6 +3955,7 @@
       <c r="F50" s="16" t="s">
         <v>321</v>
       </c>
+      <c r="G50" s="16"/>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
@@ -3964,6 +3987,7 @@
       <c r="F51" s="16" t="s">
         <v>322</v>
       </c>
+      <c r="G51" s="16"/>
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
@@ -3995,6 +4019,7 @@
       <c r="F52" s="16" t="s">
         <v>323</v>
       </c>
+      <c r="G52" s="16"/>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
@@ -4026,6 +4051,7 @@
       <c r="F53" s="16" t="s">
         <v>324</v>
       </c>
+      <c r="G53" s="16"/>
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
@@ -4057,6 +4083,7 @@
       <c r="F54" s="16" t="s">
         <v>325</v>
       </c>
+      <c r="G54" s="16"/>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
@@ -4088,6 +4115,7 @@
       <c r="F55" s="16" t="s">
         <v>326</v>
       </c>
+      <c r="G55" s="16"/>
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
@@ -4119,6 +4147,7 @@
       <c r="F56" s="16" t="s">
         <v>327</v>
       </c>
+      <c r="G56" s="16"/>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
@@ -4150,6 +4179,7 @@
       <c r="F57" s="16" t="s">
         <v>328</v>
       </c>
+      <c r="G57" s="16"/>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
@@ -4181,6 +4211,7 @@
       <c r="F58" s="16" t="s">
         <v>329</v>
       </c>
+      <c r="G58" s="16"/>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
@@ -4212,6 +4243,7 @@
       <c r="F59" s="16" t="s">
         <v>330</v>
       </c>
+      <c r="G59" s="16"/>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
@@ -4243,6 +4275,7 @@
       <c r="F60" s="16" t="s">
         <v>331</v>
       </c>
+      <c r="G60" s="16"/>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
       <c r="N60" s="15"/>
@@ -4274,6 +4307,7 @@
       <c r="F61" s="16" t="s">
         <v>332</v>
       </c>
+      <c r="G61" s="16"/>
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
       <c r="N61" s="15"/>
@@ -4305,6 +4339,7 @@
       <c r="F62" s="16" t="s">
         <v>333</v>
       </c>
+      <c r="G62" s="16"/>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
@@ -4336,6 +4371,7 @@
       <c r="F63" s="16" t="s">
         <v>334</v>
       </c>
+      <c r="G63" s="16"/>
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
@@ -4367,6 +4403,7 @@
       <c r="F64" s="16" t="s">
         <v>335</v>
       </c>
+      <c r="G64" s="16"/>
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
       <c r="N64" s="15"/>
@@ -4398,6 +4435,7 @@
       <c r="F65" s="16" t="s">
         <v>336</v>
       </c>
+      <c r="G65" s="16"/>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
@@ -4429,6 +4467,7 @@
       <c r="F66" s="16" t="s">
         <v>337</v>
       </c>
+      <c r="G66" s="16"/>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
       <c r="N66" s="15"/>
@@ -4460,6 +4499,7 @@
       <c r="F67" s="16" t="s">
         <v>338</v>
       </c>
+      <c r="G67" s="16"/>
       <c r="L67" s="15"/>
       <c r="M67" s="15"/>
       <c r="N67" s="15"/>
@@ -4491,6 +4531,7 @@
       <c r="F68" s="16" t="s">
         <v>339</v>
       </c>
+      <c r="G68" s="16"/>
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
@@ -4522,6 +4563,7 @@
       <c r="F69" s="16" t="s">
         <v>340</v>
       </c>
+      <c r="G69" s="16"/>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
@@ -4553,6 +4595,7 @@
       <c r="F70" s="16" t="s">
         <v>341</v>
       </c>
+      <c r="G70" s="16"/>
       <c r="L70" s="15"/>
       <c r="M70" s="15"/>
       <c r="N70" s="15"/>
@@ -4584,6 +4627,7 @@
       <c r="F71" s="16" t="s">
         <v>342</v>
       </c>
+      <c r="G71" s="16"/>
       <c r="L71" s="15"/>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
@@ -4615,6 +4659,7 @@
       <c r="F72" s="16" t="s">
         <v>343</v>
       </c>
+      <c r="G72" s="16"/>
       <c r="L72" s="15"/>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
@@ -4646,6 +4691,7 @@
       <c r="F73" s="16" t="s">
         <v>344</v>
       </c>
+      <c r="G73" s="16"/>
       <c r="L73" s="15"/>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
@@ -4677,6 +4723,7 @@
       <c r="F74" s="16" t="s">
         <v>345</v>
       </c>
+      <c r="G74" s="16"/>
       <c r="L74" s="15"/>
       <c r="M74" s="15"/>
       <c r="N74" s="15"/>
@@ -4708,6 +4755,7 @@
       <c r="F75" s="16" t="s">
         <v>346</v>
       </c>
+      <c r="G75" s="16"/>
       <c r="L75" s="15"/>
       <c r="M75" s="15"/>
       <c r="N75" s="15"/>
@@ -4739,6 +4787,7 @@
       <c r="F76" s="16" t="s">
         <v>347</v>
       </c>
+      <c r="G76" s="16"/>
       <c r="L76" s="15"/>
       <c r="M76" s="15"/>
       <c r="N76" s="15"/>
@@ -4770,6 +4819,7 @@
       <c r="F77" s="16" t="s">
         <v>348</v>
       </c>
+      <c r="G77" s="16"/>
       <c r="L77" s="15"/>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
@@ -4801,6 +4851,7 @@
       <c r="F78" s="16" t="s">
         <v>349</v>
       </c>
+      <c r="G78" s="16"/>
       <c r="L78" s="15"/>
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
@@ -4832,6 +4883,7 @@
       <c r="F79" s="16" t="s">
         <v>350</v>
       </c>
+      <c r="G79" s="16"/>
       <c r="L79" s="15"/>
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
@@ -4863,6 +4915,7 @@
       <c r="F80" s="16" t="s">
         <v>351</v>
       </c>
+      <c r="G80" s="16"/>
       <c r="L80" s="15"/>
       <c r="M80" s="15"/>
       <c r="N80" s="15"/>
@@ -4894,6 +4947,7 @@
       <c r="F81" s="16" t="s">
         <v>352</v>
       </c>
+      <c r="G81" s="16"/>
       <c r="L81" s="15"/>
       <c r="M81" s="15"/>
       <c r="N81" s="15"/>
@@ -4925,6 +4979,7 @@
       <c r="F82" s="16" t="s">
         <v>353</v>
       </c>
+      <c r="G82" s="16"/>
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
       <c r="N82" s="15"/>
@@ -4956,6 +5011,7 @@
       <c r="F83" s="16" t="s">
         <v>354</v>
       </c>
+      <c r="G83" s="16"/>
       <c r="L83" s="15"/>
       <c r="M83" s="15"/>
       <c r="N83" s="15"/>
@@ -4987,6 +5043,7 @@
       <c r="F84" s="16" t="s">
         <v>355</v>
       </c>
+      <c r="G84" s="16"/>
       <c r="L84" s="15"/>
       <c r="M84" s="15"/>
       <c r="N84" s="15"/>
@@ -5018,6 +5075,7 @@
       <c r="F85" s="16" t="s">
         <v>356</v>
       </c>
+      <c r="G85" s="16"/>
       <c r="L85" s="15"/>
       <c r="M85" s="15"/>
       <c r="N85" s="15"/>
@@ -5049,6 +5107,7 @@
       <c r="F86" s="16" t="s">
         <v>357</v>
       </c>
+      <c r="G86" s="16"/>
       <c r="L86" s="15"/>
       <c r="M86" s="15"/>
       <c r="N86" s="15"/>
@@ -5080,6 +5139,7 @@
       <c r="F87" s="16" t="s">
         <v>358</v>
       </c>
+      <c r="G87" s="16"/>
       <c r="L87" s="15"/>
       <c r="M87" s="15"/>
       <c r="N87" s="15"/>
@@ -5111,6 +5171,7 @@
       <c r="F88" s="16" t="s">
         <v>359</v>
       </c>
+      <c r="G88" s="16"/>
       <c r="L88" s="15"/>
       <c r="M88" s="15"/>
       <c r="N88" s="15"/>
@@ -5142,6 +5203,7 @@
       <c r="F89" s="16" t="s">
         <v>360</v>
       </c>
+      <c r="G89" s="16"/>
       <c r="L89" s="15"/>
       <c r="M89" s="15"/>
       <c r="N89" s="15"/>
@@ -5173,6 +5235,7 @@
       <c r="F90" s="16" t="s">
         <v>361</v>
       </c>
+      <c r="G90" s="16"/>
       <c r="L90" s="15"/>
       <c r="M90" s="15"/>
       <c r="N90" s="15"/>
@@ -5204,6 +5267,7 @@
       <c r="F91" s="16" t="s">
         <v>362</v>
       </c>
+      <c r="G91" s="16"/>
       <c r="L91" s="15"/>
       <c r="M91" s="15"/>
       <c r="N91" s="15"/>
@@ -5235,6 +5299,7 @@
       <c r="F92" s="16" t="s">
         <v>363</v>
       </c>
+      <c r="G92" s="16"/>
       <c r="L92" s="15"/>
       <c r="M92" s="15"/>
       <c r="N92" s="15"/>
@@ -5266,6 +5331,7 @@
       <c r="F93" s="16" t="s">
         <v>364</v>
       </c>
+      <c r="G93" s="16"/>
       <c r="L93" s="15"/>
       <c r="M93" s="15"/>
       <c r="N93" s="15"/>
@@ -5297,6 +5363,7 @@
       <c r="F94" s="16" t="s">
         <v>365</v>
       </c>
+      <c r="G94" s="16"/>
       <c r="L94" s="15"/>
       <c r="M94" s="15"/>
       <c r="N94" s="15"/>
@@ -5328,6 +5395,7 @@
       <c r="F95" s="16" t="s">
         <v>366</v>
       </c>
+      <c r="G95" s="16"/>
       <c r="L95" s="15"/>
       <c r="M95" s="15"/>
       <c r="N95" s="15"/>
@@ -5359,6 +5427,7 @@
       <c r="F96" s="16" t="s">
         <v>367</v>
       </c>
+      <c r="G96" s="16"/>
       <c r="L96" s="15"/>
       <c r="M96" s="15"/>
       <c r="N96" s="15"/>
@@ -5390,6 +5459,7 @@
       <c r="F97" s="16" t="s">
         <v>368</v>
       </c>
+      <c r="G97" s="16"/>
       <c r="L97" s="15"/>
       <c r="M97" s="15"/>
       <c r="N97" s="15"/>
@@ -5421,6 +5491,7 @@
       <c r="F98" s="16" t="s">
         <v>369</v>
       </c>
+      <c r="G98" s="16"/>
       <c r="L98" s="15"/>
       <c r="M98" s="15"/>
       <c r="N98" s="15"/>
@@ -5452,6 +5523,7 @@
       <c r="F99" s="16" t="s">
         <v>370</v>
       </c>
+      <c r="G99" s="16"/>
       <c r="L99" s="15"/>
       <c r="M99" s="15"/>
       <c r="N99" s="15"/>
@@ -5483,6 +5555,7 @@
       <c r="F100" s="16" t="s">
         <v>371</v>
       </c>
+      <c r="G100" s="16"/>
       <c r="L100" s="15"/>
       <c r="M100" s="15"/>
       <c r="N100" s="15"/>
@@ -5514,6 +5587,7 @@
       <c r="F101" s="16" t="s">
         <v>372</v>
       </c>
+      <c r="G101" s="16"/>
       <c r="L101" s="15"/>
       <c r="M101" s="15"/>
       <c r="N101" s="15"/>
@@ -5545,6 +5619,7 @@
       <c r="F102" s="16" t="s">
         <v>373</v>
       </c>
+      <c r="G102" s="16"/>
       <c r="L102" s="15"/>
       <c r="M102" s="15"/>
       <c r="N102" s="15"/>
@@ -5576,6 +5651,7 @@
       <c r="F103" s="16" t="s">
         <v>374</v>
       </c>
+      <c r="G103" s="16"/>
       <c r="L103" s="15"/>
       <c r="M103" s="15"/>
       <c r="N103" s="15"/>
@@ -5607,6 +5683,7 @@
       <c r="F104" s="16" t="s">
         <v>375</v>
       </c>
+      <c r="G104" s="16"/>
       <c r="L104" s="15"/>
       <c r="M104" s="15"/>
       <c r="N104" s="15"/>
@@ -5638,6 +5715,7 @@
       <c r="F105" s="16" t="s">
         <v>376</v>
       </c>
+      <c r="G105" s="16"/>
       <c r="L105" s="15"/>
       <c r="M105" s="15"/>
       <c r="N105" s="15"/>
@@ -5669,6 +5747,7 @@
       <c r="F106" s="16" t="s">
         <v>377</v>
       </c>
+      <c r="G106" s="16"/>
       <c r="L106" s="15"/>
       <c r="M106" s="15"/>
       <c r="N106" s="15"/>
@@ -5700,6 +5779,7 @@
       <c r="F107" s="16" t="s">
         <v>378</v>
       </c>
+      <c r="G107" s="16"/>
       <c r="L107" s="15"/>
       <c r="M107" s="15"/>
       <c r="N107" s="15"/>
@@ -5731,6 +5811,7 @@
       <c r="F108" s="16" t="s">
         <v>379</v>
       </c>
+      <c r="G108" s="16"/>
       <c r="L108" s="15"/>
       <c r="M108" s="15"/>
       <c r="N108" s="15"/>
@@ -5762,6 +5843,7 @@
       <c r="F109" s="16" t="s">
         <v>380</v>
       </c>
+      <c r="G109" s="16"/>
       <c r="L109" s="15"/>
       <c r="M109" s="15"/>
       <c r="N109" s="15"/>
@@ -5793,6 +5875,7 @@
       <c r="F110" s="16" t="s">
         <v>381</v>
       </c>
+      <c r="G110" s="16"/>
       <c r="L110" s="15"/>
       <c r="M110" s="15"/>
       <c r="N110" s="15"/>
@@ -5824,6 +5907,7 @@
       <c r="F111" s="16" t="s">
         <v>382</v>
       </c>
+      <c r="G111" s="16"/>
       <c r="L111" s="15"/>
       <c r="M111" s="15"/>
       <c r="N111" s="15"/>
@@ -5855,6 +5939,7 @@
       <c r="F112" s="16" t="s">
         <v>383</v>
       </c>
+      <c r="G112" s="16"/>
       <c r="L112" s="15"/>
       <c r="M112" s="15"/>
       <c r="N112" s="15"/>
@@ -5886,6 +5971,7 @@
       <c r="F113" s="16" t="s">
         <v>384</v>
       </c>
+      <c r="G113" s="16"/>
       <c r="L113" s="15"/>
       <c r="M113" s="15"/>
       <c r="N113" s="15"/>
@@ -5917,6 +6003,7 @@
       <c r="F114" s="16" t="s">
         <v>385</v>
       </c>
+      <c r="G114" s="16"/>
       <c r="L114" s="15"/>
       <c r="M114" s="15"/>
       <c r="N114" s="15"/>
@@ -5948,6 +6035,7 @@
       <c r="F115" s="16" t="s">
         <v>386</v>
       </c>
+      <c r="G115" s="16"/>
       <c r="L115" s="15"/>
       <c r="M115" s="15"/>
       <c r="N115" s="15"/>
@@ -5979,6 +6067,7 @@
       <c r="F116" s="16" t="s">
         <v>387</v>
       </c>
+      <c r="G116" s="16"/>
       <c r="L116" s="15"/>
       <c r="M116" s="15"/>
       <c r="N116" s="15"/>
@@ -6010,6 +6099,7 @@
       <c r="F117" s="16" t="s">
         <v>388</v>
       </c>
+      <c r="G117" s="16"/>
       <c r="L117" s="15"/>
       <c r="M117" s="15"/>
       <c r="N117" s="15"/>
@@ -6041,6 +6131,7 @@
       <c r="F118" s="16" t="s">
         <v>389</v>
       </c>
+      <c r="G118" s="16"/>
       <c r="L118" s="15"/>
       <c r="M118" s="15"/>
       <c r="N118" s="15"/>
@@ -6072,6 +6163,7 @@
       <c r="F119" s="16" t="s">
         <v>390</v>
       </c>
+      <c r="G119" s="16"/>
       <c r="L119" s="15"/>
       <c r="M119" s="15"/>
       <c r="N119" s="15"/>
@@ -6103,6 +6195,7 @@
       <c r="F120" s="16" t="s">
         <v>391</v>
       </c>
+      <c r="G120" s="16"/>
       <c r="L120" s="15"/>
       <c r="M120" s="15"/>
       <c r="N120" s="15"/>
@@ -6134,6 +6227,7 @@
       <c r="F121" s="16" t="s">
         <v>392</v>
       </c>
+      <c r="G121" s="16"/>
       <c r="L121" s="15"/>
       <c r="M121" s="15"/>
       <c r="N121" s="15"/>
@@ -6165,6 +6259,7 @@
       <c r="F122" s="16" t="s">
         <v>393</v>
       </c>
+      <c r="G122" s="16"/>
       <c r="L122" s="15"/>
       <c r="M122" s="15"/>
       <c r="N122" s="15"/>
@@ -6196,6 +6291,7 @@
       <c r="F123" s="16" t="s">
         <v>394</v>
       </c>
+      <c r="G123" s="16"/>
       <c r="L123" s="15"/>
       <c r="M123" s="15"/>
       <c r="N123" s="15"/>
@@ -6227,6 +6323,7 @@
       <c r="F124" s="16" t="s">
         <v>395</v>
       </c>
+      <c r="G124" s="16"/>
       <c r="L124" s="15"/>
       <c r="M124" s="15"/>
       <c r="N124" s="15"/>
@@ -6258,6 +6355,7 @@
       <c r="F125" s="16" t="s">
         <v>396</v>
       </c>
+      <c r="G125" s="16"/>
       <c r="L125" s="15"/>
       <c r="M125" s="15"/>
       <c r="N125" s="15"/>
@@ -6289,6 +6387,7 @@
       <c r="F126" s="16" t="s">
         <v>397</v>
       </c>
+      <c r="G126" s="16"/>
       <c r="L126" s="15"/>
       <c r="M126" s="15"/>
       <c r="N126" s="15"/>
@@ -6320,6 +6419,7 @@
       <c r="F127" s="16" t="s">
         <v>398</v>
       </c>
+      <c r="G127" s="16"/>
       <c r="L127" s="15"/>
       <c r="M127" s="15"/>
       <c r="N127" s="15"/>
@@ -6351,6 +6451,7 @@
       <c r="F128" s="16" t="s">
         <v>399</v>
       </c>
+      <c r="G128" s="16"/>
       <c r="L128" s="15"/>
       <c r="M128" s="15"/>
       <c r="N128" s="15"/>
@@ -6382,6 +6483,7 @@
       <c r="F129" s="16" t="s">
         <v>400</v>
       </c>
+      <c r="G129" s="16"/>
       <c r="L129" s="15"/>
       <c r="M129" s="15"/>
       <c r="N129" s="15"/>
@@ -6411,8 +6513,9 @@
         <v>33</v>
       </c>
       <c r="F130" s="16" t="s">
-        <v>401</v>
-      </c>
+        <v>495</v>
+      </c>
+      <c r="G130" s="16"/>
       <c r="I130" s="16"/>
       <c r="L130" s="15"/>
       <c r="M130" s="15"/>
@@ -6443,8 +6546,9 @@
         <v>33</v>
       </c>
       <c r="F131" s="16" t="s">
-        <v>402</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="G131" s="16"/>
       <c r="L131" s="15"/>
       <c r="M131" s="15"/>
       <c r="N131" s="15"/>
@@ -6474,8 +6578,9 @@
         <v>33</v>
       </c>
       <c r="F132" s="16" t="s">
-        <v>403</v>
-      </c>
+        <v>402</v>
+      </c>
+      <c r="G132" s="16"/>
       <c r="L132" s="15"/>
       <c r="M132" s="15"/>
       <c r="N132" s="15"/>
@@ -6505,8 +6610,9 @@
         <v>33</v>
       </c>
       <c r="F133" s="16" t="s">
-        <v>404</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="G133" s="16"/>
       <c r="L133" s="15"/>
       <c r="M133" s="15"/>
       <c r="N133" s="15"/>
@@ -6536,8 +6642,9 @@
         <v>33</v>
       </c>
       <c r="F134" s="16" t="s">
-        <v>405</v>
-      </c>
+        <v>404</v>
+      </c>
+      <c r="G134" s="16"/>
       <c r="L134" s="15"/>
       <c r="M134" s="15"/>
       <c r="N134" s="15"/>
@@ -6566,8 +6673,9 @@
         <v>33</v>
       </c>
       <c r="F135" s="16" t="s">
-        <v>406</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="G135" s="16"/>
       <c r="L135" s="15"/>
       <c r="M135" s="15"/>
       <c r="N135" s="15"/>
@@ -6596,8 +6704,9 @@
         <v>33</v>
       </c>
       <c r="F136" s="16" t="s">
-        <v>407</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="G136" s="16"/>
       <c r="L136" s="15"/>
       <c r="M136" s="15"/>
       <c r="N136" s="15"/>
@@ -6626,8 +6735,9 @@
         <v>33</v>
       </c>
       <c r="F137" s="16" t="s">
-        <v>408</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="G137" s="16"/>
       <c r="L137" s="15"/>
       <c r="M137" s="15"/>
       <c r="N137" s="15"/>
@@ -6656,8 +6766,9 @@
         <v>33</v>
       </c>
       <c r="F138" s="16" t="s">
-        <v>409</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="G138" s="16"/>
       <c r="L138" s="15"/>
       <c r="M138" s="15"/>
       <c r="N138" s="15"/>
@@ -6686,8 +6797,9 @@
         <v>33</v>
       </c>
       <c r="F139" s="16" t="s">
-        <v>410</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="G139" s="16"/>
       <c r="L139" s="15"/>
       <c r="M139" s="15"/>
       <c r="N139" s="15"/>
@@ -6716,8 +6828,9 @@
         <v>33</v>
       </c>
       <c r="F140" s="16" t="s">
-        <v>411</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="G140" s="16"/>
       <c r="L140" s="15"/>
       <c r="M140" s="15"/>
       <c r="N140" s="15"/>
@@ -6746,8 +6859,9 @@
         <v>33</v>
       </c>
       <c r="F141" s="16" t="s">
-        <v>412</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="G141" s="16"/>
       <c r="L141" s="15"/>
       <c r="M141" s="15"/>
       <c r="N141" s="15"/>
@@ -6776,8 +6890,9 @@
         <v>33</v>
       </c>
       <c r="F142" s="16" t="s">
-        <v>413</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="G142" s="16"/>
       <c r="L142" s="15"/>
       <c r="M142" s="15"/>
       <c r="N142" s="15"/>
@@ -6806,8 +6921,9 @@
         <v>33</v>
       </c>
       <c r="F143" s="16" t="s">
-        <v>414</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="G143" s="16"/>
       <c r="L143" s="15"/>
       <c r="M143" s="15"/>
       <c r="N143" s="15"/>
@@ -6836,8 +6952,9 @@
         <v>33</v>
       </c>
       <c r="F144" s="16" t="s">
-        <v>415</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="G144" s="16"/>
       <c r="H144" s="16"/>
       <c r="L144" s="15"/>
       <c r="M144" s="15"/>
@@ -6867,9 +6984,9 @@
         <v>33</v>
       </c>
       <c r="F145" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="G145" s="14"/>
+        <v>415</v>
+      </c>
+      <c r="G145" s="16"/>
       <c r="H145" s="15"/>
       <c r="I145" s="15"/>
       <c r="J145" s="15"/>
@@ -6901,9 +7018,9 @@
         <v>33</v>
       </c>
       <c r="F146" s="16" t="s">
-        <v>417</v>
-      </c>
-      <c r="G146" s="14"/>
+        <v>416</v>
+      </c>
+      <c r="G146" s="16"/>
       <c r="H146" s="15"/>
       <c r="I146" s="15"/>
       <c r="J146" s="15"/>
@@ -6935,9 +7052,9 @@
         <v>33</v>
       </c>
       <c r="F147" s="16" t="s">
-        <v>418</v>
-      </c>
-      <c r="G147" s="14"/>
+        <v>417</v>
+      </c>
+      <c r="G147" s="16"/>
       <c r="H147" s="15"/>
       <c r="I147" s="15"/>
       <c r="J147" s="15"/>
@@ -6969,9 +7086,9 @@
         <v>33</v>
       </c>
       <c r="F148" s="16" t="s">
-        <v>419</v>
-      </c>
-      <c r="G148" s="14"/>
+        <v>418</v>
+      </c>
+      <c r="G148" s="16"/>
       <c r="H148" s="15"/>
       <c r="I148" s="15"/>
       <c r="J148" s="15"/>
@@ -7003,9 +7120,9 @@
         <v>33</v>
       </c>
       <c r="F149" s="16" t="s">
-        <v>420</v>
-      </c>
-      <c r="G149" s="14"/>
+        <v>419</v>
+      </c>
+      <c r="G149" s="16"/>
       <c r="H149" s="15"/>
       <c r="I149" s="15"/>
       <c r="J149" s="15"/>
@@ -7037,9 +7154,9 @@
         <v>33</v>
       </c>
       <c r="F150" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="G150" s="14"/>
+        <v>420</v>
+      </c>
+      <c r="G150" s="16"/>
       <c r="H150" s="15"/>
       <c r="I150" s="15"/>
       <c r="J150" s="15"/>
@@ -7071,9 +7188,9 @@
         <v>33</v>
       </c>
       <c r="F151" s="16" t="s">
-        <v>422</v>
-      </c>
-      <c r="G151" s="14"/>
+        <v>421</v>
+      </c>
+      <c r="G151" s="16"/>
       <c r="H151" s="15"/>
       <c r="I151" s="15"/>
       <c r="J151" s="15"/>
@@ -7105,9 +7222,9 @@
         <v>33</v>
       </c>
       <c r="F152" s="16" t="s">
-        <v>423</v>
-      </c>
-      <c r="G152" s="14"/>
+        <v>422</v>
+      </c>
+      <c r="G152" s="16"/>
       <c r="H152" s="15"/>
       <c r="I152" s="15"/>
       <c r="J152" s="15"/>
@@ -7139,9 +7256,9 @@
         <v>33</v>
       </c>
       <c r="F153" s="16" t="s">
-        <v>424</v>
-      </c>
-      <c r="G153" s="14"/>
+        <v>423</v>
+      </c>
+      <c r="G153" s="16"/>
       <c r="H153" s="15"/>
       <c r="I153" s="15"/>
       <c r="J153" s="15"/>
@@ -7173,9 +7290,9 @@
         <v>33</v>
       </c>
       <c r="F154" s="16" t="s">
-        <v>425</v>
-      </c>
-      <c r="G154" s="14"/>
+        <v>424</v>
+      </c>
+      <c r="G154" s="16"/>
       <c r="H154" s="15"/>
       <c r="I154" s="15"/>
       <c r="J154" s="15"/>
@@ -7207,9 +7324,9 @@
         <v>33</v>
       </c>
       <c r="F155" s="16" t="s">
-        <v>426</v>
-      </c>
-      <c r="G155" s="14"/>
+        <v>425</v>
+      </c>
+      <c r="G155" s="16"/>
       <c r="H155" s="15"/>
       <c r="I155" s="15"/>
       <c r="J155" s="15"/>
@@ -7241,9 +7358,9 @@
         <v>33</v>
       </c>
       <c r="F156" s="16" t="s">
-        <v>427</v>
-      </c>
-      <c r="G156" s="14"/>
+        <v>426</v>
+      </c>
+      <c r="G156" s="16"/>
       <c r="H156" s="15"/>
       <c r="I156" s="15"/>
       <c r="J156" s="15"/>
@@ -7275,9 +7392,9 @@
         <v>33</v>
       </c>
       <c r="F157" s="16" t="s">
-        <v>428</v>
-      </c>
-      <c r="G157" s="14"/>
+        <v>427</v>
+      </c>
+      <c r="G157" s="16"/>
       <c r="H157" s="15"/>
       <c r="I157" s="15"/>
       <c r="J157" s="15"/>
@@ -7309,8 +7426,9 @@
         <v>33</v>
       </c>
       <c r="F158" s="16" t="s">
-        <v>429</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="G158" s="16"/>
       <c r="L158" s="15"/>
       <c r="M158" s="15"/>
       <c r="N158" s="15"/>
@@ -7339,8 +7457,9 @@
         <v>33</v>
       </c>
       <c r="F159" s="16" t="s">
-        <v>430</v>
-      </c>
+        <v>429</v>
+      </c>
+      <c r="G159" s="16"/>
       <c r="L159" s="15"/>
       <c r="M159" s="15"/>
       <c r="N159" s="15"/>
@@ -7369,8 +7488,9 @@
         <v>33</v>
       </c>
       <c r="F160" s="16" t="s">
-        <v>431</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="G160" s="16"/>
       <c r="L160" s="15"/>
       <c r="M160" s="15"/>
       <c r="N160" s="15"/>
@@ -7399,8 +7519,9 @@
         <v>33</v>
       </c>
       <c r="F161" s="16" t="s">
-        <v>432</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="G161" s="16"/>
       <c r="L161" s="15"/>
       <c r="M161" s="15"/>
       <c r="N161" s="15"/>
@@ -7429,8 +7550,9 @@
         <v>33</v>
       </c>
       <c r="F162" s="16" t="s">
-        <v>433</v>
-      </c>
+        <v>432</v>
+      </c>
+      <c r="G162" s="16"/>
       <c r="L162" s="15"/>
       <c r="M162" s="15"/>
       <c r="N162" s="15"/>
@@ -7459,8 +7581,9 @@
         <v>33</v>
       </c>
       <c r="F163" s="16" t="s">
-        <v>434</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="G163" s="16"/>
       <c r="L163" s="15"/>
       <c r="M163" s="15"/>
       <c r="N163" s="15"/>
@@ -7489,8 +7612,9 @@
         <v>33</v>
       </c>
       <c r="F164" s="16" t="s">
-        <v>435</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="G164" s="16"/>
       <c r="L164" s="15"/>
       <c r="M164" s="15"/>
       <c r="N164" s="15"/>
@@ -7519,8 +7643,9 @@
         <v>33</v>
       </c>
       <c r="F165" s="16" t="s">
-        <v>436</v>
-      </c>
+        <v>435</v>
+      </c>
+      <c r="G165" s="16"/>
       <c r="L165" s="15"/>
       <c r="M165" s="15"/>
       <c r="N165" s="15"/>
@@ -7549,8 +7674,9 @@
         <v>33</v>
       </c>
       <c r="F166" s="16" t="s">
-        <v>437</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="G166" s="16"/>
       <c r="L166" s="15"/>
       <c r="M166" s="15"/>
       <c r="N166" s="15"/>
@@ -7579,8 +7705,9 @@
         <v>33</v>
       </c>
       <c r="F167" s="16" t="s">
-        <v>438</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="G167" s="16"/>
       <c r="L167" s="15"/>
       <c r="M167" s="15"/>
       <c r="N167" s="15"/>
@@ -7609,8 +7736,9 @@
         <v>33</v>
       </c>
       <c r="F168" s="16" t="s">
-        <v>439</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="G168" s="16"/>
       <c r="L168" s="15"/>
       <c r="M168" s="15"/>
       <c r="N168" s="15"/>
@@ -7639,8 +7767,9 @@
         <v>33</v>
       </c>
       <c r="F169" s="16" t="s">
-        <v>440</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="G169" s="16"/>
       <c r="L169" s="15"/>
       <c r="M169" s="15"/>
       <c r="N169" s="15"/>
@@ -7669,8 +7798,9 @@
         <v>33</v>
       </c>
       <c r="F170" s="16" t="s">
-        <v>441</v>
-      </c>
+        <v>440</v>
+      </c>
+      <c r="G170" s="16"/>
       <c r="L170" s="15"/>
       <c r="M170" s="15"/>
       <c r="N170" s="15"/>
@@ -7699,8 +7829,9 @@
         <v>33</v>
       </c>
       <c r="F171" s="16" t="s">
-        <v>442</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="G171" s="16"/>
       <c r="L171" s="15"/>
       <c r="M171" s="15"/>
       <c r="N171" s="15"/>
@@ -7729,8 +7860,9 @@
         <v>33</v>
       </c>
       <c r="F172" s="16" t="s">
-        <v>443</v>
-      </c>
+        <v>442</v>
+      </c>
+      <c r="G172" s="16"/>
       <c r="L172" s="15"/>
       <c r="M172" s="15"/>
       <c r="N172" s="15"/>
@@ -7759,8 +7891,9 @@
         <v>33</v>
       </c>
       <c r="F173" s="16" t="s">
-        <v>444</v>
-      </c>
+        <v>443</v>
+      </c>
+      <c r="G173" s="16"/>
       <c r="L173" s="15"/>
       <c r="M173" s="15"/>
       <c r="N173" s="15"/>
@@ -7789,8 +7922,9 @@
         <v>33</v>
       </c>
       <c r="F174" s="16" t="s">
-        <v>445</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="G174" s="16"/>
       <c r="L174" s="15"/>
       <c r="M174" s="15"/>
       <c r="N174" s="15"/>
@@ -7819,8 +7953,9 @@
         <v>33</v>
       </c>
       <c r="F175" s="16" t="s">
-        <v>446</v>
-      </c>
+        <v>445</v>
+      </c>
+      <c r="G175" s="16"/>
       <c r="L175" s="15"/>
       <c r="M175" s="15"/>
       <c r="N175" s="15"/>
@@ -7849,8 +7984,9 @@
         <v>33</v>
       </c>
       <c r="F176" s="16" t="s">
-        <v>447</v>
-      </c>
+        <v>446</v>
+      </c>
+      <c r="G176" s="16"/>
       <c r="L176" s="15"/>
       <c r="M176" s="15"/>
       <c r="N176" s="15"/>
@@ -7879,8 +8015,9 @@
         <v>33</v>
       </c>
       <c r="F177" s="16" t="s">
-        <v>448</v>
-      </c>
+        <v>447</v>
+      </c>
+      <c r="G177" s="16"/>
       <c r="L177" s="15"/>
       <c r="M177" s="15"/>
       <c r="N177" s="15"/>
@@ -7909,8 +8046,9 @@
         <v>33</v>
       </c>
       <c r="F178" s="16" t="s">
-        <v>449</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="G178" s="16"/>
       <c r="L178" s="15"/>
       <c r="M178" s="15"/>
       <c r="N178" s="15"/>
@@ -7939,8 +8077,9 @@
         <v>33</v>
       </c>
       <c r="F179" s="16" t="s">
-        <v>450</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="G179" s="16"/>
       <c r="L179" s="15"/>
       <c r="M179" s="15"/>
       <c r="N179" s="15"/>
@@ -7969,8 +8108,9 @@
         <v>33</v>
       </c>
       <c r="F180" s="16" t="s">
-        <v>451</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="G180" s="16"/>
       <c r="L180" s="15"/>
       <c r="M180" s="15"/>
       <c r="N180" s="15"/>
@@ -7999,8 +8139,9 @@
         <v>33</v>
       </c>
       <c r="F181" s="16" t="s">
-        <v>452</v>
-      </c>
+        <v>451</v>
+      </c>
+      <c r="G181" s="16"/>
       <c r="L181" s="15"/>
       <c r="M181" s="15"/>
       <c r="N181" s="15"/>
@@ -8029,8 +8170,9 @@
         <v>33</v>
       </c>
       <c r="F182" s="16" t="s">
-        <v>453</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="G182" s="16"/>
       <c r="L182" s="15"/>
       <c r="M182" s="15"/>
       <c r="N182" s="15"/>
@@ -8059,8 +8201,9 @@
         <v>33</v>
       </c>
       <c r="F183" s="16" t="s">
-        <v>454</v>
-      </c>
+        <v>453</v>
+      </c>
+      <c r="G183" s="16"/>
       <c r="L183" s="15"/>
       <c r="M183" s="15"/>
       <c r="N183" s="15"/>
@@ -8089,8 +8232,9 @@
         <v>33</v>
       </c>
       <c r="F184" s="16" t="s">
-        <v>455</v>
-      </c>
+        <v>454</v>
+      </c>
+      <c r="G184" s="16"/>
       <c r="L184" s="15"/>
       <c r="M184" s="15"/>
       <c r="N184" s="15"/>
@@ -8119,8 +8263,9 @@
         <v>33</v>
       </c>
       <c r="F185" s="16" t="s">
-        <v>456</v>
-      </c>
+        <v>455</v>
+      </c>
+      <c r="G185" s="16"/>
       <c r="L185" s="15"/>
       <c r="M185" s="15"/>
       <c r="N185" s="15"/>
@@ -8149,8 +8294,9 @@
         <v>33</v>
       </c>
       <c r="F186" s="16" t="s">
-        <v>457</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="G186" s="16"/>
       <c r="L186" s="15"/>
       <c r="M186" s="15"/>
       <c r="N186" s="15"/>
@@ -8179,8 +8325,9 @@
         <v>33</v>
       </c>
       <c r="F187" s="16" t="s">
-        <v>458</v>
-      </c>
+        <v>457</v>
+      </c>
+      <c r="G187" s="16"/>
       <c r="L187" s="15"/>
       <c r="M187" s="15"/>
       <c r="N187" s="15"/>
@@ -8209,8 +8356,9 @@
         <v>33</v>
       </c>
       <c r="F188" s="16" t="s">
-        <v>459</v>
-      </c>
+        <v>458</v>
+      </c>
+      <c r="G188" s="16"/>
       <c r="L188" s="15"/>
       <c r="M188" s="15"/>
       <c r="N188" s="15"/>
@@ -8239,8 +8387,9 @@
         <v>33</v>
       </c>
       <c r="F189" s="16" t="s">
-        <v>460</v>
-      </c>
+        <v>459</v>
+      </c>
+      <c r="G189" s="16"/>
       <c r="L189" s="15"/>
       <c r="M189" s="15"/>
       <c r="N189" s="15"/>
@@ -8269,8 +8418,9 @@
         <v>33</v>
       </c>
       <c r="F190" s="16" t="s">
-        <v>461</v>
-      </c>
+        <v>460</v>
+      </c>
+      <c r="G190" s="16"/>
       <c r="L190" s="15"/>
       <c r="M190" s="15"/>
       <c r="N190" s="15"/>
@@ -8299,8 +8449,9 @@
         <v>33</v>
       </c>
       <c r="F191" s="16" t="s">
-        <v>462</v>
-      </c>
+        <v>461</v>
+      </c>
+      <c r="G191" s="16"/>
       <c r="L191" s="15"/>
       <c r="M191" s="15"/>
       <c r="N191" s="15"/>
@@ -8329,8 +8480,9 @@
         <v>33</v>
       </c>
       <c r="F192" s="16" t="s">
-        <v>463</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="G192" s="16"/>
       <c r="L192" s="15"/>
       <c r="M192" s="15"/>
       <c r="N192" s="15"/>
@@ -8359,8 +8511,9 @@
         <v>33</v>
       </c>
       <c r="F193" s="16" t="s">
-        <v>464</v>
-      </c>
+        <v>463</v>
+      </c>
+      <c r="G193" s="16"/>
       <c r="L193" s="15"/>
       <c r="M193" s="15"/>
       <c r="N193" s="15"/>
@@ -8389,8 +8542,9 @@
         <v>33</v>
       </c>
       <c r="F194" s="16" t="s">
-        <v>465</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="G194" s="16"/>
       <c r="L194" s="15"/>
       <c r="M194" s="15"/>
       <c r="N194" s="15"/>
@@ -8419,8 +8573,9 @@
         <v>33</v>
       </c>
       <c r="F195" s="16" t="s">
-        <v>466</v>
-      </c>
+        <v>465</v>
+      </c>
+      <c r="G195" s="16"/>
       <c r="L195" s="15"/>
       <c r="M195" s="15"/>
       <c r="N195" s="15"/>
@@ -8449,8 +8604,9 @@
         <v>33</v>
       </c>
       <c r="F196" s="16" t="s">
-        <v>467</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="G196" s="16"/>
       <c r="L196" s="15"/>
       <c r="M196" s="15"/>
       <c r="N196" s="15"/>
@@ -8479,8 +8635,9 @@
         <v>33</v>
       </c>
       <c r="F197" s="16" t="s">
-        <v>468</v>
-      </c>
+        <v>467</v>
+      </c>
+      <c r="G197" s="16"/>
       <c r="L197" s="15"/>
       <c r="M197" s="15"/>
       <c r="N197" s="15"/>
@@ -8509,8 +8666,9 @@
         <v>33</v>
       </c>
       <c r="F198" s="16" t="s">
-        <v>469</v>
-      </c>
+        <v>468</v>
+      </c>
+      <c r="G198" s="16"/>
       <c r="I198" s="15">
         <v>1</v>
       </c>
@@ -8566,8 +8724,9 @@
         <v>33</v>
       </c>
       <c r="F199" s="16" t="s">
-        <v>470</v>
-      </c>
+        <v>469</v>
+      </c>
+      <c r="G199" s="16"/>
       <c r="H199" s="15">
         <v>1</v>
       </c>
@@ -8624,8 +8783,9 @@
         <v>33</v>
       </c>
       <c r="F200" s="16" t="s">
-        <v>471</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="G200" s="16"/>
       <c r="H200" s="15">
         <v>1</v>
       </c>
@@ -8682,8 +8842,9 @@
         <v>33</v>
       </c>
       <c r="F201" s="16" t="s">
-        <v>472</v>
-      </c>
+        <v>471</v>
+      </c>
+      <c r="G201" s="16"/>
       <c r="L201" s="15"/>
       <c r="M201" s="15"/>
       <c r="N201" s="15"/>
@@ -8712,8 +8873,9 @@
         <v>33</v>
       </c>
       <c r="F202" s="16" t="s">
-        <v>473</v>
-      </c>
+        <v>472</v>
+      </c>
+      <c r="G202" s="16"/>
       <c r="L202" s="15"/>
       <c r="M202" s="15"/>
       <c r="N202" s="15"/>
@@ -8742,8 +8904,9 @@
         <v>33</v>
       </c>
       <c r="F203" s="16" t="s">
-        <v>474</v>
-      </c>
+        <v>473</v>
+      </c>
+      <c r="G203" s="16"/>
       <c r="L203" s="15"/>
       <c r="M203" s="15"/>
       <c r="N203" s="15"/>
@@ -8766,7 +8929,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8973,7 +9136,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B2" s="15">
         <v>3</v>
@@ -8990,7 +9153,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B3" s="15">
         <v>4</v>
@@ -9007,7 +9170,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B4" s="15">
         <v>2</v>
@@ -9024,7 +9187,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B5" s="15">
         <v>4</v>
@@ -9041,7 +9204,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B6" s="15">
         <v>4</v>
@@ -9058,7 +9221,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B7" s="15">
         <v>4</v>
@@ -9075,7 +9238,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B8" s="15">
         <v>3</v>
@@ -9092,7 +9255,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B9" s="15">
         <v>4</v>
@@ -9109,7 +9272,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B10" s="15">
         <v>2</v>
@@ -9126,7 +9289,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B11" s="15">
         <v>4</v>
@@ -9143,7 +9306,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B12" s="15">
         <v>4</v>
@@ -9217,52 +9380,52 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -9288,37 +9451,37 @@
     <row r="1" spans="1:14" s="21" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>475</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>476</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>477</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>478</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>479</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>480</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>481</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>482</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>483</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>484</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>485</v>
       </c>
       <c r="M1" s="21" t="s">
         <v>30</v>
@@ -10076,34 +10239,34 @@
     <row r="1" spans="1:24" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20"/>
       <c r="B1" s="21" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>486</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>487</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>488</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>489</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>490</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>491</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>492</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>493</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>494</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>495</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -11551,34 +11714,34 @@
     <row r="1" spans="1:24" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20"/>
       <c r="B1" s="21" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>486</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>487</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>488</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>494</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>495</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -11596,57 +11759,57 @@
     </row>
     <row r="2" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="10.199999999999999" x14ac:dyDescent="0.3">

</xml_diff>